<commit_message>
user schema id 변경
</commit_message>
<xml_diff>
--- a/resource/API.xlsx
+++ b/resource/API.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\carpool_git\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7174FE-71F7-449D-9FB0-52E5A5F1B7BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="135">
   <si>
     <t>url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -114,10 +115,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>사람 이름</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>식별자</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -285,10 +282,6 @@
     <t>table 이름</t>
   </si>
   <si>
-    <t>* memberID/memberPW 값은 통합 로그인이 완성되기 전까지 임시로 사용한다. 통합 로그인이 완성되면 그때 session id를 받아오든 해야 한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>users_and_rooms_infos</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -550,13 +543,32 @@
   </si>
   <si>
     <t>http request pbody에 roomID를 넘겨줌. 기능은 위와 동일.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>memberEmail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>memberType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>token에 있는 정보</t>
+  </si>
+  <si>
+    <t>token에 있는 정보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>식별자(token에 있는 정보)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1163,31 +1175,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="130.59765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.3984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.09765625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.59765625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.3984375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23.69921875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="130.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.75" style="1" customWidth="1"/>
     <col min="8" max="8" width="29.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.59765625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.3984375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.3984375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.19921875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.25" style="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1204,7 +1216,7 @@
       <c r="K1" s="24"/>
       <c r="L1" s="12"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -1212,358 +1224,364 @@
         <v>17</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15"/>
       <c r="B3" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D3" s="29" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>22</v>
+        <v>133</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="16"/>
-    </row>
-    <row r="4" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+        <v>30</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="15"/>
       <c r="L4" s="16"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L5" s="16"/>
     </row>
-    <row r="6" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15"/>
       <c r="B6" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="9"/>
       <c r="L6" s="16"/>
     </row>
-    <row r="7" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="15"/>
       <c r="B7" s="17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D7" s="15"/>
       <c r="L7" s="16"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="15"/>
       <c r="B8" s="16"/>
       <c r="D8" s="31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L8" s="16"/>
     </row>
-    <row r="9" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>20</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>27</v>
-      </c>
       <c r="L9" s="16"/>
     </row>
-    <row r="10" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="15"/>
       <c r="B10" s="16"/>
       <c r="D10" s="15"/>
       <c r="L10" s="16"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L11" s="25" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="I12" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L12" s="26" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D13" s="15"/>
       <c r="G13" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="L13" s="16"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L14" s="16"/>
     </row>
-    <row r="15" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>20</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L15" s="16"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="16" t="s">
         <v>104</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>106</v>
       </c>
       <c r="D16" s="18"/>
       <c r="L16" s="16"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="L17" s="16"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="2"/>
       <c r="L18" s="16"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="2"/>
       <c r="L19" s="16"/>
     </row>
-    <row r="20" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D20" s="19"/>
       <c r="E20" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F20" s="28"/>
       <c r="G20" s="28"/>
@@ -1573,143 +1591,143 @@
       <c r="K20" s="28"/>
       <c r="L20" s="20"/>
     </row>
-    <row r="21" spans="1:12" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D22" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E22" s="30" t="s">
+      <c r="G22" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A23" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.4">
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B24" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25"/>
       <c r="B25" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="15"/>
       <c r="B26" s="17"/>
       <c r="G26" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.4">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="18" thickTop="1" x14ac:dyDescent="0.4"/>
-    <row r="33" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="34" spans="1:2" ht="18" thickTop="1" x14ac:dyDescent="0.4">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="34" spans="1:2" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B34" s="21"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
         <v>5</v>
       </c>
@@ -1717,95 +1735,95 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
         <v>9</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="15" t="s">
         <v>14</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="18" thickTop="1" x14ac:dyDescent="0.4"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="17.25" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>